<commit_message>
added separate page for survey and recommendation
</commit_message>
<xml_diff>
--- a/WIBDSoulSister/Survey.xlsx
+++ b/WIBDSoulSister/Survey.xlsx
@@ -1,44 +1,70 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>Flying first class</t>
+  </si>
+  <si>
+    <t>6am-12pm</t>
+  </si>
+  <si>
+    <t>Twitter</t>
+  </si>
+  <si>
+    <t>Procrastination</t>
+  </si>
+  <si>
+    <t>shreya.pradhan@womeninbigdata.asia</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <i val="1"/>
-      <color theme="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <scheme val="minor"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -53,85 +79,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -419,194 +384,92 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="A1:XFD1048576"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col width="9.140625" customWidth="1" style="1" min="1" max="16384"/>
+    <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>jdjdkjdksjdks</t>
-        </is>
+    <row r="1" spans="1:5">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Self-doubt</t>
-        </is>
+      <c r="B1" t="s">
+        <v>3</v>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Flying first class</t>
-        </is>
+      <c r="C1" t="s">
+        <v>0</v>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>6am-12pm</t>
-        </is>
+      <c r="D1" t="s">
+        <v>1</v>
       </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Twitter</t>
-        </is>
+      <c r="E1" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>jdjdkjdksjdks</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Self-doubt</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Flying first class</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>6am-12pm</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Twitter</t>
-        </is>
-      </c>
+    <row r="2" spans="1:5">
+      <c r="A2"/>
+      <c r="B2"/>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>jdjdkjdksjdks</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Self-doubt</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Flying first class</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>12pm-6pm</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Twitter</t>
-        </is>
-      </c>
+    <row r="3" spans="1:5">
+      <c r="A3"/>
+      <c r="B3"/>
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="E3"/>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>jdjdkjdksjdks</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Self-doubt</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Flying first class</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>12pm-6pm</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Facebook</t>
-        </is>
-      </c>
+    <row r="4" spans="1:5">
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="C4"/>
+      <c r="D4"/>
+      <c r="E4"/>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>new</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Procrastination</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Flying first class</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>6am-12pm</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Twitter</t>
-        </is>
-      </c>
+    <row r="5" spans="1:5">
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="E5"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>